<commit_message>
rows met no changes verwijderd
</commit_message>
<xml_diff>
--- a/zib2017-2020/mapping/excel/Adresgegevens.xlsx
+++ b/zib2017-2020/mapping/excel/Adresgegevens.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindamook/Documents/GitHub/nictiz/Zibtranslate/zib2017-2020/mapping/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53DF606-6603-6D4B-8561-25A6E68C3FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">translations!$A$1:$O$14</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
   <si>
     <t>ZibName</t>
   </si>
@@ -162,9 +168,6 @@
   </si>
   <si>
     <t>Typo in engelse tekst in waarde binnen AdresTypeCodelijst aangepast. "Tempory address" moet zijn "Temporary address"</t>
-  </si>
-  <si>
-    <t>NO CHANGE</t>
   </si>
   <si>
     <t>CARDINALITY CHANGE</t>
@@ -188,8 +191,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,7 +257,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA003"/>
         </patternFill>
       </fill>
     </dxf>
@@ -268,26 +278,27 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFA003"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -325,7 +336,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -359,6 +370,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -393,9 +405,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -568,21 +581,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="15" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="5" width="40.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="15" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +642,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -648,11 +661,8 @@
       <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -671,11 +681,8 @@
       <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -694,11 +701,8 @@
       <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -717,11 +721,8 @@
       <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="K5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -746,11 +747,8 @@
       <c r="H6" t="s">
         <v>39</v>
       </c>
-      <c r="K6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -769,11 +767,8 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="K7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -792,11 +787,8 @@
       <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="K8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -828,22 +820,22 @@
         <v>46</v>
       </c>
       <c r="K9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
         <v>51</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>52</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>53</v>
       </c>
-      <c r="O9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -875,16 +867,16 @@
         <v>47</v>
       </c>
       <c r="K10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" t="s">
         <v>50</v>
       </c>
-      <c r="L10" t="s">
-        <v>51</v>
-      </c>
       <c r="N10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -903,11 +895,8 @@
       <c r="G11" t="s">
         <v>35</v>
       </c>
-      <c r="K11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -932,11 +921,8 @@
       <c r="H12" t="s">
         <v>41</v>
       </c>
-      <c r="K12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -955,11 +941,8 @@
       <c r="G13" t="s">
         <v>37</v>
       </c>
-      <c r="K13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -978,23 +961,20 @@
       <c r="G14" t="s">
         <v>38</v>
       </c>
-      <c r="K14" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O14"/>
+  <autoFilter ref="A1:O14" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="E2:E14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"groen: geen wijzigingen"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"geel: patch wijziging"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"oranje: minor change"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"rood: major change"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>